<commit_message>
Updated phase 1 analysis
</commit_message>
<xml_diff>
--- a/correlation_results.xlsx
+++ b/correlation_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\candy\OneDrive\Desktop\FireHua Consulting LLC\Data Projects\Data Project 1 - HR Analytics Dashboard Employee Attrition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\candy\OneDrive\Desktop\FireHua Consulting LLC\Data Projects\employee-attrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD9776-8E14-4449-B946-BCC1EDC2F915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA11DBAC-03CB-4CFD-9F65-BD9FBB7D832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All correlations" sheetId="5" r:id="rId1"/>
@@ -415,7 +415,10 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -429,12 +432,37 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-66EA-4187-98B2-614752DFC7FA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -448,12 +476,37 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-5384-4F4C-A603-C7A1D912F093}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -463,6 +516,28 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-66EA-4187-98B2-614752DFC7FA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-5384-4F4C-A603-C7A1D912F093}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -494,10 +569,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -516,10 +588,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -538,10 +607,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -560,10 +626,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -582,10 +645,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -604,10 +664,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -622,36 +679,6 @@
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="0"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-66EA-4187-98B2-614752DFC7FA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-66EA-4187-98B2-614752DFC7FA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
               <c:idx val="6"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -663,6 +690,36 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-66EA-4187-98B2-614752DFC7FA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-66EA-4187-98B2-614752DFC7FA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-66EA-4187-98B2-614752DFC7FA}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -727,43 +784,43 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>Over Time</c:v>
+                  <c:v>Relationship Satisfaction</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Education</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Years Since Last Promotion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Percent Salary Hike</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Work Life Balance</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Environment Satisfaction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Job Satisfaction</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Stock Option Level</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Total Satisfaction Score</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Age</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Monthly Income</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Total Working Years</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Age</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Monthly Income</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Total Satisfaction Score</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Stock Option Level</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Environment Satisfaction</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Job Satisfaction</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Work Life Balance</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Percent Salary Hike</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Education</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Years Since Last Promotion</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>Relationship Satisfaction</c:v>
+                  <c:v>Over Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -775,43 +832,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.17</c:v>
+                  <c:v>-0.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.16</c:v>
+                  <c:v>-0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.16</c:v>
+                  <c:v>-0.01</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.15</c:v>
+                  <c:v>-0.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.14000000000000001</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.06</c:v>
+                  <c:v>-0.15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.01</c:v>
+                  <c:v>-0.16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.03</c:v>
+                  <c:v>-0.16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.03</c:v>
+                  <c:v>-0.17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.05</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,15 +1587,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>906427</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>36857</xdr:rowOff>
+      <xdr:colOff>881580</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>111401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>184559</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>139127</xdr:rowOff>
+      <xdr:colOff>159712</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>23171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1568,7 +1625,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3184144" y="4989857"/>
+          <a:off x="3159297" y="5577923"/>
           <a:ext cx="189219" cy="1245270"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1591,9 +1648,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>728869</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>74543</xdr:rowOff>
+      <xdr:colOff>704022</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1618713" cy="248851"/>
     <xdr:sp macro="" textlink="">
@@ -1609,7 +1666,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3006586" y="4588565"/>
+          <a:off x="2981739" y="5234609"/>
           <a:ext cx="1618713" cy="248851"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1667,15 +1724,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>240195</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>149086</xdr:rowOff>
+      <xdr:colOff>215348</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>587237</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>110986</xdr:rowOff>
+      <xdr:colOff>562390</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>185530</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1705,7 +1762,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3428999" y="4762499"/>
+          <a:off x="3404152" y="5499652"/>
           <a:ext cx="959955" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1728,15 +1785,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>231913</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>132519</xdr:rowOff>
+      <xdr:colOff>207066</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>16563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>94419</xdr:rowOff>
+      <xdr:colOff>556178</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>168963</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1766,7 +1823,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3420717" y="5126932"/>
+          <a:off x="3395870" y="5864085"/>
           <a:ext cx="962025" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1789,15 +1846,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>240195</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>115957</xdr:rowOff>
+      <xdr:colOff>215348</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>583509</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>77857</xdr:rowOff>
+      <xdr:colOff>558662</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1827,7 +1884,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3428999" y="5491370"/>
+          <a:off x="3404152" y="6228523"/>
           <a:ext cx="956227" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1850,15 +1907,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>231914</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66260</xdr:rowOff>
+      <xdr:colOff>207067</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>140804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>190085</xdr:rowOff>
+      <xdr:colOff>556179</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>74129</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1888,7 +1945,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3420718" y="5913782"/>
+          <a:off x="3395871" y="6559826"/>
           <a:ext cx="962025" cy="314325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2198,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9744E6A6-5E8B-47DB-8740-F278C5CA9C07}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,154 +2291,154 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3">
-        <v>0.25</v>
+        <v>-0.05</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>7.8710000000000002E-2</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G10" si="0">ABS(C2)</f>
-        <v>0.25</v>
+        <f>-ABS(C2)</f>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>-0.17</v>
+        <v>-0.03</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>0.22932</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>0.17</v>
+        <f>-ABS(C3)</f>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
-        <v>-0.16</v>
+        <v>-0.03</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>0.20579</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>-ABS(C4)</f>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>-0.16</v>
+        <v>-0.01</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>0.60560999999999998</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>-ABS(C5)</f>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
-        <v>-0.15</v>
+        <v>-0.06</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>1.421E-2</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+        <f t="shared" ref="G6:G14" si="0">ABS(C6)</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3">
-        <v>-0.14000000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
         <v>-0.1</v>
@@ -2393,7 +2450,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -2406,51 +2463,51 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.1</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>6.9999999999999994E-5</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.06</v>
+        <v>-0.15</v>
       </c>
       <c r="D10" s="2">
-        <v>1.421E-2</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
       <c r="H10" s="7"/>
       <c r="J10" s="10" t="s">
@@ -2459,51 +2516,51 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3">
-        <v>-0.01</v>
+        <v>-0.16</v>
       </c>
       <c r="D11" s="2">
-        <v>0.60560999999999998</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <f>-ABS(C11)</f>
-        <v>-0.01</v>
+        <f t="shared" si="0"/>
+        <v>0.16</v>
       </c>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>-0.03</v>
+        <v>-0.16</v>
       </c>
       <c r="D12" s="2">
-        <v>0.22932</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <f>-ABS(C12)</f>
-        <v>-0.03</v>
+        <f t="shared" si="0"/>
+        <v>0.16</v>
       </c>
       <c r="H12" s="6"/>
       <c r="J12" s="10" t="s">
@@ -2512,51 +2569,51 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C13" s="3">
-        <v>-0.03</v>
+        <v>-0.17</v>
       </c>
       <c r="D13" s="2">
-        <v>0.20579</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13">
-        <f>-ABS(C13)</f>
-        <v>-0.03</v>
+        <f t="shared" si="0"/>
+        <v>0.17</v>
       </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3">
-        <v>-0.05</v>
+        <v>0.25</v>
       </c>
       <c r="D14" s="2">
-        <v>7.8710000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <f>-ABS(C14)</f>
-        <v>-0.05</v>
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="H14" s="5"/>
       <c r="J14" s="10" t="s">
@@ -2565,7 +2622,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
-    <sortCondition descending="1" ref="G2:G14"/>
+    <sortCondition ref="G2:G14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>